<commit_message>
Updated after team Review
</commit_message>
<xml_diff>
--- a/test_controls_enhanced_modules_analysis_results.xlsx
+++ b/test_controls_enhanced_modules_analysis_results.xlsx
@@ -450,7 +450,7 @@
     <col width="37.40000000000001" customWidth="1" min="5" max="5"/>
     <col width="14.3" customWidth="1" min="6" max="6"/>
     <col width="12.1" customWidth="1" min="7" max="7"/>
-    <col width="20.9" customWidth="1" min="8" max="8"/>
+    <col width="13.2" customWidth="1" min="8" max="8"/>
     <col width="22" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="10" max="10"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -579,7 +579,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>86.06</v>
+        <v>87.16</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -600,7 +600,7 @@
         <v>120</v>
       </c>
       <c r="H2" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I2" t="n">
         <v>74</v>
@@ -643,7 +643,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description matches metadata (monthly)</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -669,7 +669,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>75.58</v>
+        <v>76.68000000000001</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -690,7 +690,7 @@
         <v>90</v>
       </c>
       <c r="H3" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I3" t="n">
         <v>74</v>
@@ -729,7 +729,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description matches metadata (monthly)</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -810,12 +810,12 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (monthly)</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -841,7 +841,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>28.8</v>
+        <v>46.40000000000001</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -850,7 +850,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WHEN, WHAT, WHY, ESCALATION</t>
+          <t>WHAT, WHY, ESCALATION</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -862,7 +862,7 @@
         <v>90</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -896,12 +896,12 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (ongoing)</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -927,7 +927,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>25.6</v>
+        <v>43.2</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -936,7 +936,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>WHEN, WHAT, WHY, ESCALATION</t>
+          <t>WHAT, WHY, ESCALATION</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -948,7 +948,7 @@
         <v>80</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -982,12 +982,12 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (daily)</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1072,12 +1072,12 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (monthly)</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1158,12 +1158,12 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (as needed)</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1244,12 +1244,12 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (quarterly)</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1330,12 +1330,12 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (weekly)</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -1420,12 +1420,12 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (monthly)</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -1451,7 +1451,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>28.74544</v>
+        <v>29.84544</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1472,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I12" t="n">
         <v>31.392</v>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description matches metadata (monthly)</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>45.58</v>
+        <v>46.68</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1558,7 +1558,7 @@
         <v>84</v>
       </c>
       <c r="H13" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description matches metadata (weekly)</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -1623,7 +1623,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>47.545</v>
+        <v>45.40000000000001</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1644,7 +1644,7 @@
         <v>80</v>
       </c>
       <c r="H14" t="n">
-        <v>99.75000000000001</v>
+        <v>90</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description matches metadata (quarterly)</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>Vague timing detected</t>
+          <t>Frequency in description (none) does not match metadata (as needed)</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
@@ -1795,7 +1795,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>33.465</v>
+        <v>30.22</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1816,7 +1816,7 @@
         <v>36</v>
       </c>
       <c r="H16" t="n">
-        <v>99.75</v>
+        <v>85</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1850,12 +1850,12 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (within 3 days)</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -1940,12 +1940,12 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (ongoing)</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -2026,12 +2026,12 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (regulatory)</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -2112,12 +2112,12 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (ongoing)</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
@@ -2198,12 +2198,12 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (prompt)</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
@@ -2284,12 +2284,12 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description (none) does not match metadata (internal)</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
@@ -2401,7 +2401,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>74.46000000000001</v>
+        <v>52.68</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>WHY</t>
+          <t>WHEN, WHY</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2422,7 +2422,7 @@
         <v>80</v>
       </c>
       <c r="H23" t="n">
-        <v>99.00000000000001</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
         <v>74</v>
@@ -2745,7 +2745,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>95.16000000000001</v>
+        <v>93.18000000000001</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -2766,7 +2766,7 @@
         <v>120</v>
       </c>
       <c r="H27" t="n">
-        <v>99.00000000000001</v>
+        <v>90</v>
       </c>
       <c r="I27" t="n">
         <v>80</v>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description matches metadata (daily)</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
@@ -2831,7 +2831,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>90.74111359999999</v>
+        <v>91.8411136</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -2852,7 +2852,7 @@
         <v>120</v>
       </c>
       <c r="H28" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I28" t="n">
         <v>88.62848</v>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description matches metadata (monthly, quarterly)</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -2917,7 +2917,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>87.98</v>
+        <v>89.08</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -2938,7 +2938,7 @@
         <v>120</v>
       </c>
       <c r="H29" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I29" t="n">
         <v>80</v>
@@ -2956,13 +2956,13 @@
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>high</t>
         </is>
       </c>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description matches metadata (weekly, ad hoc)</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
@@ -3003,7 +3003,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>82.163488</v>
+        <v>83.263488</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -3024,7 +3024,7 @@
         <v>120</v>
       </c>
       <c r="H30" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I30" t="n">
         <v>80.19839999999999</v>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description matches metadata (daily)</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -3093,7 +3093,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>94.16173217391304</v>
+        <v>95.26173217391305</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -3114,7 +3114,7 @@
         <v>120</v>
       </c>
       <c r="H31" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I31" t="n">
         <v>99.31791304347827</v>
@@ -3153,7 +3153,7 @@
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>No frequency metadata provided for validation</t>
+          <t>Frequency in description matches metadata (weekly, monthly)</t>
         </is>
       </c>
       <c r="S31" t="inlineStr">
@@ -3188,7 +3188,7 @@
   <cols>
     <col width="13.2" customWidth="1" min="1" max="1"/>
     <col width="26.4" customWidth="1" min="2" max="2"/>
-    <col width="48.40000000000001" customWidth="1" min="3" max="3"/>
+    <col width="29.7" customWidth="1" min="3" max="3"/>
     <col width="50" customWidth="1" min="4" max="4"/>
     <col width="50" customWidth="1" min="5" max="5"/>
     <col width="50" customWidth="1" min="6" max="6"/>
@@ -3335,7 +3335,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>by the infosec team</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3367,7 +3367,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>by the finance team bef</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3559,7 +3559,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>monthly, on a monthly basis, monthly basis</t>
+          <t>on a monthly basis</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>when an employee leaves, quarterly</t>
+          <t>quarterly</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -3655,7 +3655,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>exceptions are addressed as needed</t>
+          <t>as needed</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -3815,7 +3815,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>promptly</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -3911,7 +3911,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>when exceptions are found</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>if discrepancies are found, daily</t>
+          <t>daily</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -4103,7 +4103,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>weekly, on a weekly basis, weekly basis</t>
+          <t>ad hoc, on a weekly basis</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -4286,7 +4286,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (Monthly)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>Align the frequency in the description with the declared frequency (Ongoing)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -4338,7 +4338,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>Align the frequency in the description with the declared frequency (Daily)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -4362,7 +4362,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (Monthly)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -4386,7 +4386,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (As needed)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -4414,7 +4414,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (Quarterly)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -4442,7 +4442,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (Weekly)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (Monthly)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -4558,7 +4558,7 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Replace vague term 'exceptions are addressed as needed' with specific frequency (daily, weekly, monthly).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Replace vague timing term 'as needed' with a specific timeframe or frequency.; Align the frequency in the description with the declared frequency (As needed)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -4584,7 +4584,11 @@
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Align the frequency in the description with the declared frequency (Within 3 days)</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>No clear control action detected. Add a specific verb describing what the control does.</t>
@@ -4610,7 +4614,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (Ongoing)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -4634,7 +4638,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (Regulatory)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -4662,7 +4666,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (Ongoing)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -4690,7 +4694,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Replace vague timing term 'promptly' with specific timeframe (e.g., 'within 24 hours').</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (Prompt)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -4722,7 +4726,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Align the frequency in the description with the declared frequency (Internal)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -4768,7 +4772,11 @@
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
@@ -4912,7 +4920,11 @@
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>While 'ad-hoc' is an allowed frequency, the control would be stronger if it specified what triggers the ad-hoc review.; Multiple frequencies detected. Consider whether this is describing a process rather than a single control.</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>Consider specifying WHERE the control is performed (system, application, or location)</t>
@@ -5079,7 +5091,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>41.8</t>
+          <t>42.3</t>
         </is>
       </c>
     </row>
@@ -5171,7 +5183,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>18 (60.0%)</t>
+          <t>17 (56.7%)</t>
         </is>
       </c>
     </row>
@@ -5255,7 +5267,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>29 (96.7%)</t>
+          <t>15 (50.0%)</t>
         </is>
       </c>
     </row>
@@ -5267,7 +5279,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1 (3.3%)</t>
+          <t>15 (50.0%)</t>
         </is>
       </c>
     </row>

</xml_diff>